<commit_message>
Changes lsit u pdate
</commit_message>
<xml_diff>
--- a/Changes.xlsx
+++ b/Changes.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="changes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">changes!$B$1:$B$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">changes!$A$1:$C$35</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,12 +211,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -233,12 +227,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -522,11 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +539,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -565,11 +557,11 @@
       <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -587,11 +579,11 @@
       <c r="B5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -609,11 +601,11 @@
       <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -635,7 +627,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -657,7 +649,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -679,7 +671,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -701,15 +693,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>39</v>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -723,15 +715,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>39</v>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,15 +737,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>39</v>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,15 +759,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>39</v>
+      <c r="C22" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -789,15 +781,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>39</v>
+      <c r="C24" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -811,15 +803,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>39</v>
+      <c r="C26" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,7 +825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -855,7 +847,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -877,7 +869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -899,7 +891,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -922,13 +914,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B35">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Sami"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C35">
       <formula1>"Pending, Development, Completed"</formula1>

</xml_diff>